<commit_message>
changes to duplicates1 2 and codebook
</commit_message>
<xml_diff>
--- a/_overlaps_feb_2020_final.xlsx
+++ b/_overlaps_feb_2020_final.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X25"/>
+  <dimension ref="A1:X23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -666,7 +666,7 @@
         </is>
       </c>
       <c r="G4">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -691,7 +691,7 @@
         <v>42720</v>
       </c>
       <c r="O4" s="2">
-        <v>42859</v>
+        <v>42856</v>
       </c>
       <c r="P4">
         <v>205</v>
@@ -700,7 +700,7 @@
         <v>1054</v>
       </c>
       <c r="R4">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="U4" t="inlineStr">
         <is>
@@ -711,7 +711,7 @@
         <v>17151</v>
       </c>
       <c r="W4">
-        <v>17290</v>
+        <v>17287</v>
       </c>
       <c r="X4">
         <v>0</v>
@@ -738,7 +738,7 @@
         </is>
       </c>
       <c r="G5">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -1083,7 +1083,7 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>JUCA1**061955</t>
+          <t>JUCA1**071955</t>
         </is>
       </c>
       <c r="M9" s="2">
@@ -1394,7 +1394,7 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>FRCA1**071985</t>
+          <t>FAMU2**071985</t>
         </is>
       </c>
       <c r="M13" s="2">
@@ -1625,58 +1625,80 @@
       <c r="B16">
         <v>1</v>
       </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
       <c r="D16">
         <v>0</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="F16">
+        <v>1</v>
       </c>
       <c r="G16">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="H16">
         <v>0</v>
       </c>
       <c r="I16">
-        <v>25303</v>
+        <v>26804</v>
       </c>
       <c r="J16">
         <v>2012</v>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>1d53b9a82ab4fbc0e6cfa109d664eb51</t>
+          <t>5fab3d3029d511f60544d7a58d047e5c</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>12G10**61993</t>
-        </is>
+          <t>GABE2**081978</t>
+        </is>
+      </c>
+      <c r="M16" s="2">
+        <v>41240</v>
       </c>
       <c r="N16" s="2">
-        <v>40987</v>
+        <v>41053</v>
       </c>
       <c r="O16" s="2">
-        <v>41187</v>
+        <v>41238</v>
+      </c>
+      <c r="P16">
+        <v>146</v>
       </c>
       <c r="Q16">
-        <v>2787</v>
+        <v>187</v>
       </c>
       <c r="R16">
-        <v>200</v>
+        <v>185</v>
+      </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>Derivación</t>
+        </is>
+      </c>
+      <c r="T16" t="inlineStr">
+        <is>
+          <t>Derivación</t>
+        </is>
       </c>
       <c r="U16" t="inlineStr">
         <is>
-          <t>PG-PAI</t>
+          <t>PG-PAB</t>
         </is>
       </c>
       <c r="V16">
-        <v>15418</v>
+        <v>15484</v>
       </c>
       <c r="W16">
-        <v>15618</v>
+        <v>15669</v>
       </c>
       <c r="X16">
         <v>0</v>
@@ -1691,71 +1713,80 @@
       <c r="B17">
         <v>2</v>
       </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
       <c r="D17">
         <v>0</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="F17">
+        <v>1</v>
       </c>
       <c r="G17">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="H17">
         <v>0</v>
       </c>
       <c r="I17">
-        <v>29037</v>
+        <v>31405</v>
       </c>
       <c r="J17">
         <v>2012</v>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>1d53b9a82ab4fbc0e6cfa109d664eb51</t>
+          <t>5fab3d3029d511f60544d7a58d047e5c</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>12G10**61993</t>
+          <t>GABE2**081978</t>
         </is>
       </c>
       <c r="M17" s="2">
-        <v>41289</v>
+        <v>41260</v>
       </c>
       <c r="N17" s="2">
-        <v>41141</v>
+        <v>41207</v>
       </c>
       <c r="O17" s="2">
-        <v>41289</v>
+        <v>41238</v>
+      </c>
+      <c r="P17">
+        <v>142</v>
       </c>
       <c r="Q17">
-        <v>148</v>
+        <v>53</v>
       </c>
       <c r="R17">
-        <v>148</v>
+        <v>31</v>
       </c>
       <c r="S17" t="inlineStr">
         <is>
-          <t>Derivación</t>
+          <t>Alta Terapéutica</t>
         </is>
       </c>
       <c r="T17" t="inlineStr">
         <is>
-          <t>Derivación</t>
+          <t>Alta Terapéutica</t>
         </is>
       </c>
       <c r="U17" t="inlineStr">
         <is>
-          <t>Otro</t>
+          <t>PG-PR</t>
         </is>
       </c>
       <c r="V17">
-        <v>15572</v>
+        <v>15638</v>
       </c>
       <c r="W17">
-        <v>15720</v>
+        <v>15669</v>
       </c>
       <c r="X17">
         <v>0</v>
@@ -1774,76 +1805,60 @@
         <v>0</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
       </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
       <c r="G18">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="H18">
         <v>0</v>
       </c>
       <c r="I18">
-        <v>26804</v>
+        <v>18784</v>
       </c>
       <c r="J18">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>5fab3d3029d511f60544d7a58d047e5c</t>
+          <t>0d7fe0ff18f5b16868a68ca5ee5d4b87</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>GABE2**081978</t>
-        </is>
-      </c>
-      <c r="M18" s="2">
-        <v>41240</v>
+          <t>CEOR1**051979</t>
+        </is>
       </c>
       <c r="N18" s="2">
-        <v>41053</v>
+        <v>40792</v>
       </c>
       <c r="O18" s="2">
-        <v>41238</v>
+        <v>40920</v>
       </c>
       <c r="P18">
-        <v>146</v>
+        <v>308</v>
       </c>
       <c r="Q18">
-        <v>187</v>
+        <v>2982</v>
       </c>
       <c r="R18">
-        <v>185</v>
-      </c>
-      <c r="S18" t="inlineStr">
-        <is>
-          <t>Derivación</t>
-        </is>
-      </c>
-      <c r="T18" t="inlineStr">
-        <is>
-          <t>Derivación</t>
-        </is>
+        <v>128</v>
       </c>
       <c r="U18" t="inlineStr">
         <is>
-          <t>PG-PAB</t>
+          <t>PG-PR</t>
         </is>
       </c>
       <c r="V18">
-        <v>15484</v>
+        <v>15223</v>
       </c>
       <c r="W18">
-        <v>15669</v>
+        <v>15351</v>
       </c>
       <c r="X18">
         <v>0</v>
@@ -1862,76 +1877,73 @@
         <v>0</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Si</t>
-        </is>
-      </c>
-      <c r="F19">
-        <v>1</v>
+          <t>No</t>
+        </is>
       </c>
       <c r="G19">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="H19">
         <v>0</v>
       </c>
       <c r="I19">
-        <v>31405</v>
+        <v>24395</v>
       </c>
       <c r="J19">
         <v>2012</v>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>5fab3d3029d511f60544d7a58d047e5c</t>
+          <t>0d7fe0ff18f5b16868a68ca5ee5d4b87</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>GABE2**081978</t>
+          <t>CEOR1**051979</t>
         </is>
       </c>
       <c r="M19" s="2">
-        <v>41260</v>
+        <v>41001</v>
       </c>
       <c r="N19" s="2">
-        <v>41207</v>
+        <v>40918</v>
       </c>
       <c r="O19" s="2">
-        <v>41238</v>
+        <v>41001</v>
       </c>
       <c r="P19">
-        <v>142</v>
+        <v>309</v>
       </c>
       <c r="Q19">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="R19">
-        <v>31</v>
+        <v>83</v>
       </c>
       <c r="S19" t="inlineStr">
         <is>
-          <t>Alta Terapéutica</t>
+          <t>Abandono</t>
         </is>
       </c>
       <c r="T19" t="inlineStr">
         <is>
-          <t>Alta Terapéutica</t>
+          <t>Abandono</t>
         </is>
       </c>
       <c r="U19" t="inlineStr">
         <is>
-          <t>PG-PR</t>
+          <t>PG-PAI</t>
         </is>
       </c>
       <c r="V19">
-        <v>15638</v>
+        <v>15349</v>
       </c>
       <c r="W19">
-        <v>15669</v>
+        <v>15432</v>
       </c>
       <c r="X19">
         <v>0</v>
@@ -1954,59 +1966,75 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Si</t>
-        </is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F20">
+        <v>0</v>
       </c>
       <c r="G20">
-        <v>2</v>
+        <v>2069</v>
       </c>
       <c r="H20">
         <v>0</v>
       </c>
       <c r="I20">
-        <v>18784</v>
+        <v>826</v>
       </c>
       <c r="J20">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>0d7fe0ff18f5b16868a68ca5ee5d4b87</t>
+          <t>584feda92f394aa23d89e5162b8e3d05</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>CEOR1**051979</t>
-        </is>
+          <t>LUCA1**121957</t>
+        </is>
+      </c>
+      <c r="M20" s="2">
+        <v>42370</v>
       </c>
       <c r="N20" s="2">
-        <v>40792</v>
+        <v>39948</v>
       </c>
       <c r="O20" s="2">
-        <v>40920</v>
+        <v>42370</v>
       </c>
       <c r="P20">
-        <v>308</v>
+        <v>128</v>
       </c>
       <c r="Q20">
-        <v>2982</v>
+        <v>2422</v>
       </c>
       <c r="R20">
-        <v>128</v>
+        <v>2422</v>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>Alta Admnistrativa</t>
+        </is>
+      </c>
+      <c r="T20" t="inlineStr">
+        <is>
+          <t>Alta Admnistrativa</t>
+        </is>
       </c>
       <c r="U20" t="inlineStr">
         <is>
-          <t>PG-PR</t>
+          <t>PG-PAB</t>
         </is>
       </c>
       <c r="V20">
-        <v>15223</v>
+        <v>14379</v>
       </c>
       <c r="W20">
-        <v>15351</v>
+        <v>16801</v>
       </c>
       <c r="X20">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
@@ -2029,69 +2057,72 @@
           <t>No</t>
         </is>
       </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
       <c r="G21">
-        <v>2</v>
+        <v>2069</v>
       </c>
       <c r="H21">
         <v>0</v>
       </c>
       <c r="I21">
-        <v>24395</v>
+        <v>20689</v>
       </c>
       <c r="J21">
         <v>2012</v>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>0d7fe0ff18f5b16868a68ca5ee5d4b87</t>
+          <t>584feda92f394aa23d89e5162b8e3d05</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>CEOR1**051979</t>
+          <t>LUCA1**121957</t>
         </is>
       </c>
       <c r="M21" s="2">
-        <v>41001</v>
+        <v>41274</v>
       </c>
       <c r="N21" s="2">
-        <v>40918</v>
+        <v>40301</v>
       </c>
       <c r="O21" s="2">
-        <v>41001</v>
+        <v>41274</v>
       </c>
       <c r="P21">
-        <v>309</v>
+        <v>127</v>
       </c>
       <c r="Q21">
-        <v>83</v>
+        <v>973</v>
       </c>
       <c r="R21">
-        <v>83</v>
+        <v>973</v>
       </c>
       <c r="S21" t="inlineStr">
         <is>
-          <t>Abandono</t>
+          <t>Derivación</t>
         </is>
       </c>
       <c r="T21" t="inlineStr">
         <is>
-          <t>Abandono</t>
+          <t>Derivación</t>
         </is>
       </c>
       <c r="U21" t="inlineStr">
         <is>
-          <t>PG-PAI</t>
+          <t>PG-PR</t>
         </is>
       </c>
       <c r="V21">
-        <v>15349</v>
+        <v>14732</v>
       </c>
       <c r="W21">
-        <v>15432</v>
+        <v>15705</v>
       </c>
       <c r="X21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
@@ -2104,82 +2135,76 @@
         <v>1</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Si</t>
         </is>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22">
-        <v>2069</v>
+        <v>191</v>
       </c>
       <c r="H22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22">
-        <v>826</v>
+        <v>6868</v>
       </c>
       <c r="J22">
         <v>2010</v>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>584feda92f394aa23d89e5162b8e3d05</t>
+          <t>91d2b53989232617a76554f9df52348c</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>LUCA1**121957</t>
-        </is>
-      </c>
-      <c r="M22" s="2">
-        <v>42370</v>
+          <t>JUTI1**011982</t>
+        </is>
       </c>
       <c r="N22" s="2">
-        <v>39948</v>
+        <v>40360</v>
       </c>
       <c r="O22" s="2">
-        <v>42370</v>
+        <v>40556</v>
       </c>
       <c r="P22">
-        <v>128</v>
-      </c>
-      <c r="Q22">
-        <v>2422</v>
+        <v>109</v>
       </c>
       <c r="R22">
-        <v>2422</v>
+        <v>196</v>
       </c>
       <c r="S22" t="inlineStr">
         <is>
-          <t>Alta Admnistrativa</t>
+          <t>Derivación</t>
         </is>
       </c>
       <c r="T22" t="inlineStr">
         <is>
-          <t>Alta Admnistrativa</t>
+          <t>Derivación</t>
         </is>
       </c>
       <c r="U22" t="inlineStr">
         <is>
-          <t>PG-PAB</t>
+          <t>PG-PAI</t>
         </is>
       </c>
       <c r="V22">
-        <v>14379</v>
+        <v>14791</v>
       </c>
       <c r="W22">
-        <v>16801</v>
+        <v>14987</v>
       </c>
       <c r="X22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -2192,251 +2217,81 @@
         <v>2</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Si</t>
         </is>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23">
-        <v>2069</v>
+        <v>191</v>
       </c>
       <c r="H23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23">
-        <v>20689</v>
+        <v>7566</v>
       </c>
       <c r="J23">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>584feda92f394aa23d89e5162b8e3d05</t>
+          <t>91d2b53989232617a76554f9df52348c</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>LUCA1**121957</t>
+          <t>JUTI1**011982</t>
         </is>
       </c>
       <c r="M23" s="2">
-        <v>41274</v>
+        <v>40740</v>
       </c>
       <c r="N23" s="2">
-        <v>40301</v>
+        <v>40365</v>
       </c>
       <c r="O23" s="2">
-        <v>41274</v>
+        <v>40740</v>
       </c>
       <c r="P23">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="Q23">
-        <v>973</v>
+        <v>375</v>
       </c>
       <c r="R23">
-        <v>973</v>
+        <v>375</v>
       </c>
       <c r="S23" t="inlineStr">
         <is>
-          <t>Derivación</t>
+          <t>Alta Admnistrativa</t>
         </is>
       </c>
       <c r="T23" t="inlineStr">
         <is>
-          <t>Derivación</t>
+          <t>Alta Admnistrativa</t>
         </is>
       </c>
       <c r="U23" t="inlineStr">
         <is>
-          <t>PG-PR</t>
+          <t>PG-PAI</t>
         </is>
       </c>
       <c r="V23">
-        <v>14732</v>
+        <v>14796</v>
       </c>
       <c r="W23">
-        <v>15705</v>
+        <v>15171</v>
       </c>
       <c r="X23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>Si</t>
-        </is>
-      </c>
-      <c r="F24">
-        <v>1</v>
-      </c>
-      <c r="G24">
-        <v>191</v>
-      </c>
-      <c r="H24">
-        <v>1</v>
-      </c>
-      <c r="I24">
-        <v>6868</v>
-      </c>
-      <c r="J24">
-        <v>2010</v>
-      </c>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>91d2b53989232617a76554f9df52348c</t>
-        </is>
-      </c>
-      <c r="L24" t="inlineStr">
-        <is>
-          <t>JUTI1**071982</t>
-        </is>
-      </c>
-      <c r="N24" s="2">
-        <v>40360</v>
-      </c>
-      <c r="O24" s="2">
-        <v>40556</v>
-      </c>
-      <c r="P24">
-        <v>109</v>
-      </c>
-      <c r="R24">
-        <v>196</v>
-      </c>
-      <c r="S24" t="inlineStr">
-        <is>
-          <t>Derivación</t>
-        </is>
-      </c>
-      <c r="T24" t="inlineStr">
-        <is>
-          <t>Derivación</t>
-        </is>
-      </c>
-      <c r="U24" t="inlineStr">
-        <is>
-          <t>PG-PAI</t>
-        </is>
-      </c>
-      <c r="V24">
-        <v>14791</v>
-      </c>
-      <c r="W24">
-        <v>14987</v>
-      </c>
-      <c r="X24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="B25">
-        <v>2</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>Si</t>
-        </is>
-      </c>
-      <c r="F25">
-        <v>1</v>
-      </c>
-      <c r="G25">
-        <v>191</v>
-      </c>
-      <c r="H25">
-        <v>1</v>
-      </c>
-      <c r="I25">
-        <v>7566</v>
-      </c>
-      <c r="J25">
-        <v>2010</v>
-      </c>
-      <c r="K25" t="inlineStr">
-        <is>
-          <t>91d2b53989232617a76554f9df52348c</t>
-        </is>
-      </c>
-      <c r="L25" t="inlineStr">
-        <is>
-          <t>JUTI1**071982</t>
-        </is>
-      </c>
-      <c r="M25" s="2">
-        <v>40740</v>
-      </c>
-      <c r="N25" s="2">
-        <v>40365</v>
-      </c>
-      <c r="O25" s="2">
-        <v>40740</v>
-      </c>
-      <c r="P25">
-        <v>109</v>
-      </c>
-      <c r="Q25">
-        <v>375</v>
-      </c>
-      <c r="R25">
-        <v>375</v>
-      </c>
-      <c r="S25" t="inlineStr">
-        <is>
-          <t>Alta Admnistrativa</t>
-        </is>
-      </c>
-      <c r="T25" t="inlineStr">
-        <is>
-          <t>Alta Admnistrativa</t>
-        </is>
-      </c>
-      <c r="U25" t="inlineStr">
-        <is>
-          <t>PG-PAI</t>
-        </is>
-      </c>
-      <c r="V25">
-        <v>14796</v>
-      </c>
-      <c r="W25">
-        <v>15171</v>
-      </c>
-      <c r="X25">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changes to duplicates3, sex, pregnancy & such
</commit_message>
<xml_diff>
--- a/_overlaps_feb_2020_final.xlsx
+++ b/_overlaps_feb_2020_final.xlsx
@@ -498,7 +498,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -508,56 +508,72 @@
           <t>Si</t>
         </is>
       </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
       <c r="G2">
-        <v>71</v>
+        <v>31</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
-        <v>157931</v>
+        <v>26804</v>
       </c>
       <c r="J2">
-        <v>2019</v>
+        <v>2012</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>a92ab8f10fa05d0d9dcb5855c0ec0092</t>
+          <t>5fab3d3029d511f60544d7a58d047e5c</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>RITR1**111984</t>
-        </is>
+          <t>GABE2**081978</t>
+        </is>
+      </c>
+      <c r="M2" s="2">
+        <v>41240</v>
       </c>
       <c r="N2" s="2">
-        <v>43579</v>
+        <v>41053</v>
       </c>
       <c r="O2" s="2">
-        <v>43669</v>
+        <v>41238</v>
       </c>
       <c r="P2">
-        <v>291</v>
+        <v>146</v>
       </c>
       <c r="Q2">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="R2">
-        <v>90</v>
+        <v>185</v>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>Derivación</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>Derivación</t>
+        </is>
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>PG-PAI</t>
+          <t>PG-PAB</t>
         </is>
       </c>
       <c r="V2">
-        <v>18010</v>
+        <v>15484</v>
       </c>
       <c r="W2">
-        <v>18100</v>
+        <v>15669</v>
       </c>
       <c r="X2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -570,7 +586,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -580,69 +596,72 @@
           <t>Si</t>
         </is>
       </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
       <c r="G3">
-        <v>71</v>
+        <v>31</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>156785</v>
+        <v>31405</v>
       </c>
       <c r="J3">
-        <v>2019</v>
+        <v>2012</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>a92ab8f10fa05d0d9dcb5855c0ec0092</t>
+          <t>5fab3d3029d511f60544d7a58d047e5c</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>RITR1**111984</t>
+          <t>GABE2**081978</t>
         </is>
       </c>
       <c r="M3" s="2">
-        <v>43607</v>
+        <v>41260</v>
       </c>
       <c r="N3" s="2">
-        <v>43598</v>
+        <v>41207</v>
       </c>
       <c r="O3" s="2">
-        <v>43607</v>
+        <v>41238</v>
       </c>
       <c r="P3">
-        <v>291</v>
+        <v>142</v>
       </c>
       <c r="Q3">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="R3">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>Abandono</t>
+          <t>Alta Terapéutica</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>Abandono</t>
+          <t>Alta Terapéutica</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>M-PAI</t>
+          <t>PG-PR</t>
         </is>
       </c>
       <c r="V3">
-        <v>18029</v>
+        <v>15638</v>
       </c>
       <c r="W3">
-        <v>18038</v>
+        <v>15669</v>
       </c>
       <c r="X3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -665,53 +684,69 @@
           <t>Si</t>
         </is>
       </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
       <c r="G4">
-        <v>90</v>
+        <v>6</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
       <c r="I4">
-        <v>111197</v>
+        <v>36873</v>
       </c>
       <c r="J4">
-        <v>2017</v>
+        <v>2013</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>144b8d70d7ea1b9ea70d2ef7543520b2</t>
+          <t>953090fd0a141e1cb79c86c7b209009f</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>OSBE1**061978</t>
-        </is>
+          <t>JOPA1**031985</t>
+        </is>
+      </c>
+      <c r="M4" s="2">
+        <v>41449</v>
       </c>
       <c r="N4" s="2">
-        <v>42720</v>
+        <v>41295</v>
       </c>
       <c r="O4" s="2">
-        <v>42856</v>
+        <v>41437</v>
       </c>
       <c r="P4">
-        <v>205</v>
+        <v>155</v>
       </c>
       <c r="Q4">
-        <v>1054</v>
+        <v>154</v>
       </c>
       <c r="R4">
-        <v>136</v>
+        <v>142</v>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>Abandono</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>Abandono</t>
+        </is>
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>PG-PAI</t>
+          <t>PG-PAB</t>
         </is>
       </c>
       <c r="V4">
-        <v>17151</v>
+        <v>15726</v>
       </c>
       <c r="W4">
-        <v>17287</v>
+        <v>15868</v>
       </c>
       <c r="X4">
         <v>0</v>
@@ -737,66 +772,69 @@
           <t>Si</t>
         </is>
       </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
       <c r="G5">
-        <v>90</v>
+        <v>6</v>
       </c>
       <c r="H5">
         <v>1</v>
       </c>
       <c r="I5">
-        <v>112951</v>
+        <v>42419</v>
       </c>
       <c r="J5">
-        <v>2017</v>
+        <v>2013</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>144b8d70d7ea1b9ea70d2ef7543520b2</t>
+          <t>953090fd0a141e1cb79c86c7b209009f</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>OSBE1**061978</t>
+          <t>JOPA1**031985</t>
         </is>
       </c>
       <c r="M5" s="2">
-        <v>43038</v>
+        <v>41607</v>
       </c>
       <c r="N5" s="2">
-        <v>42766</v>
+        <v>41431</v>
       </c>
       <c r="O5" s="2">
-        <v>43038</v>
+        <v>41607</v>
       </c>
       <c r="P5">
-        <v>682</v>
+        <v>254</v>
       </c>
       <c r="Q5">
-        <v>272</v>
+        <v>176</v>
       </c>
       <c r="R5">
-        <v>272</v>
+        <v>176</v>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>Alta Terapéutica</t>
+          <t>Alta Admnistrativa</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>Alta Terapéutica</t>
+          <t>Alta Admnistrativa</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>PG-PR</t>
+          <t>PG-PAI</t>
         </is>
       </c>
       <c r="V5">
-        <v>17197</v>
+        <v>15862</v>
       </c>
       <c r="W5">
-        <v>17469</v>
+        <v>16038</v>
       </c>
       <c r="X5">
         <v>0</v>
@@ -812,7 +850,7 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -823,41 +861,41 @@
         </is>
       </c>
       <c r="G6">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
-        <v>109317</v>
+        <v>157931</v>
       </c>
       <c r="J6">
-        <v>2017</v>
+        <v>2019</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>1baff032eb17af74d98d63542c87423a</t>
+          <t>a92ab8f10fa05d0d9dcb5855c0ec0092</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>CEME1**081985</t>
+          <t>RITR1**111984</t>
         </is>
       </c>
       <c r="N6" s="2">
-        <v>42626</v>
+        <v>43579</v>
       </c>
       <c r="O6" s="2">
-        <v>42785</v>
+        <v>43669</v>
       </c>
       <c r="P6">
-        <v>205</v>
+        <v>291</v>
       </c>
       <c r="Q6">
-        <v>1148</v>
+        <v>203</v>
       </c>
       <c r="R6">
-        <v>159</v>
+        <v>90</v>
       </c>
       <c r="U6" t="inlineStr">
         <is>
@@ -865,10 +903,10 @@
         </is>
       </c>
       <c r="V6">
-        <v>17057</v>
+        <v>18010</v>
       </c>
       <c r="W6">
-        <v>17216</v>
+        <v>18100</v>
       </c>
       <c r="X6">
         <v>1</v>
@@ -884,7 +922,7 @@
         <v>2</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -895,65 +933,65 @@
         </is>
       </c>
       <c r="G7">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7">
-        <v>112950</v>
+        <v>156785</v>
       </c>
       <c r="J7">
-        <v>2017</v>
+        <v>2019</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>1baff032eb17af74d98d63542c87423a</t>
+          <t>a92ab8f10fa05d0d9dcb5855c0ec0092</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>CEME1**081985</t>
+          <t>RITR1**111984</t>
         </is>
       </c>
       <c r="M7" s="2">
-        <v>42775</v>
+        <v>43607</v>
       </c>
       <c r="N7" s="2">
-        <v>42762</v>
+        <v>43598</v>
       </c>
       <c r="O7" s="2">
-        <v>42775</v>
+        <v>43607</v>
       </c>
       <c r="P7">
-        <v>682</v>
+        <v>291</v>
       </c>
       <c r="Q7">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="R7">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>Alta Admnistrativa</t>
+          <t>Abandono</t>
         </is>
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>Alta Admnistrativa</t>
+          <t>Abandono</t>
         </is>
       </c>
       <c r="U7" t="inlineStr">
         <is>
-          <t>PG-PR</t>
+          <t>M-PAI</t>
         </is>
       </c>
       <c r="V7">
-        <v>17193</v>
+        <v>18029</v>
       </c>
       <c r="W7">
-        <v>17206</v>
+        <v>18038</v>
       </c>
       <c r="X7">
         <v>1</v>
@@ -968,6 +1006,9 @@
       <c r="B8">
         <v>1</v>
       </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
       <c r="D8">
         <v>0</v>
       </c>
@@ -976,58 +1017,42 @@
           <t>Si</t>
         </is>
       </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
       <c r="G8">
-        <v>511</v>
+        <v>90</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8">
-        <v>86673</v>
+        <v>111197</v>
       </c>
       <c r="J8">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>380d9b27915ca8873d06f71d4d74030e</t>
+          <t>144b8d70d7ea1b9ea70d2ef7543520b2</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>JUCA1**071955</t>
-        </is>
-      </c>
-      <c r="M8" s="2">
-        <v>42458</v>
+          <t>OSBE1**061978</t>
+        </is>
       </c>
       <c r="N8" s="2">
-        <v>41939</v>
+        <v>42720</v>
       </c>
       <c r="O8" s="2">
-        <v>42458</v>
+        <v>42856</v>
       </c>
       <c r="P8">
-        <v>105</v>
+        <v>205</v>
       </c>
       <c r="Q8">
-        <v>519</v>
+        <v>1054</v>
       </c>
       <c r="R8">
-        <v>519</v>
-      </c>
-      <c r="S8" t="inlineStr">
-        <is>
-          <t>Alta Terapéutica</t>
-        </is>
-      </c>
-      <c r="T8" t="inlineStr">
-        <is>
-          <t>Alta Terapéutica</t>
-        </is>
+        <v>136</v>
       </c>
       <c r="U8" t="inlineStr">
         <is>
@@ -1035,13 +1060,13 @@
         </is>
       </c>
       <c r="V8">
-        <v>16370</v>
+        <v>17151</v>
       </c>
       <c r="W8">
-        <v>16889</v>
+        <v>17287</v>
       </c>
       <c r="X8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -1053,6 +1078,9 @@
       <c r="B9">
         <v>2</v>
       </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
       <c r="D9">
         <v>0</v>
       </c>
@@ -1061,69 +1089,69 @@
           <t>Si</t>
         </is>
       </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
       <c r="G9">
-        <v>511</v>
+        <v>90</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9">
-        <v>64530</v>
+        <v>112951</v>
       </c>
       <c r="J9">
-        <v>2014</v>
+        <v>2017</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>380d9b27915ca8873d06f71d4d74030e</t>
+          <t>144b8d70d7ea1b9ea70d2ef7543520b2</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>JUCA1**071955</t>
+          <t>OSBE1**061978</t>
         </is>
       </c>
       <c r="M9" s="2">
-        <v>41948</v>
+        <v>43038</v>
       </c>
       <c r="N9" s="2">
-        <v>41947</v>
+        <v>42766</v>
       </c>
       <c r="O9" s="2">
-        <v>41948</v>
+        <v>43038</v>
+      </c>
+      <c r="P9">
+        <v>682</v>
       </c>
       <c r="Q9">
-        <v>1</v>
+        <v>272</v>
       </c>
       <c r="R9">
-        <v>1</v>
+        <v>272</v>
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>Alta Admnistrativa</t>
+          <t>Alta Terapéutica</t>
         </is>
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>Alta Admnistrativa</t>
+          <t>Alta Terapéutica</t>
         </is>
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>CALLE</t>
+          <t>PG-PR</t>
         </is>
       </c>
       <c r="V9">
-        <v>16378</v>
+        <v>17197</v>
       </c>
       <c r="W9">
-        <v>16379</v>
+        <v>17469</v>
       </c>
       <c r="X9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -1136,7 +1164,7 @@
         <v>1</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1147,55 +1175,55 @@
         </is>
       </c>
       <c r="G10">
-        <v>88</v>
+        <v>23</v>
       </c>
       <c r="H10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10">
-        <v>89750</v>
+        <v>109317</v>
       </c>
       <c r="J10">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>a91ebc49e725f0638be44c6e17445adb</t>
+          <t>1baff032eb17af74d98d63542c87423a</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>BACA1**071992</t>
+          <t>CEME1**081985</t>
         </is>
       </c>
       <c r="N10" s="2">
-        <v>42270</v>
+        <v>42626</v>
       </c>
       <c r="O10" s="2">
-        <v>42366</v>
+        <v>42785</v>
       </c>
       <c r="P10">
-        <v>167</v>
+        <v>205</v>
       </c>
       <c r="Q10">
-        <v>1504</v>
+        <v>1148</v>
       </c>
       <c r="R10">
-        <v>96</v>
+        <v>159</v>
       </c>
       <c r="U10" t="inlineStr">
         <is>
-          <t>PG-PR</t>
+          <t>PG-PAI</t>
         </is>
       </c>
       <c r="V10">
-        <v>16701</v>
+        <v>17057</v>
       </c>
       <c r="W10">
-        <v>16797</v>
+        <v>17216</v>
       </c>
       <c r="X10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -1208,7 +1236,7 @@
         <v>2</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1219,53 +1247,53 @@
         </is>
       </c>
       <c r="G11">
-        <v>88</v>
+        <v>23</v>
       </c>
       <c r="H11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11">
-        <v>94274</v>
+        <v>112950</v>
       </c>
       <c r="J11">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>a91ebc49e725f0638be44c6e17445adb</t>
+          <t>1baff032eb17af74d98d63542c87423a</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>BACA1**071992</t>
+          <t>CEME1**081985</t>
         </is>
       </c>
       <c r="M11" s="2">
-        <v>42475</v>
+        <v>42775</v>
       </c>
       <c r="N11" s="2">
-        <v>42278</v>
+        <v>42762</v>
       </c>
       <c r="O11" s="2">
-        <v>42475</v>
+        <v>42775</v>
       </c>
       <c r="P11">
-        <v>167</v>
+        <v>682</v>
       </c>
       <c r="Q11">
-        <v>197</v>
+        <v>13</v>
       </c>
       <c r="R11">
-        <v>197</v>
+        <v>13</v>
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>Abandono</t>
+          <t>Alta Admnistrativa</t>
         </is>
       </c>
       <c r="T11" t="inlineStr">
         <is>
-          <t>Abandono</t>
+          <t>Alta Admnistrativa</t>
         </is>
       </c>
       <c r="U11" t="inlineStr">
@@ -1274,13 +1302,13 @@
         </is>
       </c>
       <c r="V11">
-        <v>16709</v>
+        <v>17193</v>
       </c>
       <c r="W11">
-        <v>16906</v>
+        <v>17206</v>
       </c>
       <c r="X11">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -1292,9 +1320,6 @@
       <c r="B12">
         <v>1</v>
       </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
       <c r="D12">
         <v>0</v>
       </c>
@@ -1303,56 +1328,72 @@
           <t>Si</t>
         </is>
       </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
       <c r="G12">
-        <v>214</v>
+        <v>511</v>
       </c>
       <c r="H12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I12">
-        <v>65674</v>
+        <v>86673</v>
       </c>
       <c r="J12">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>137e8525aa3f79235fa8ad90913fdcbe</t>
+          <t>380d9b27915ca8873d06f71d4d74030e</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>FRCA1**071985</t>
-        </is>
+          <t>JUCA1**071955</t>
+        </is>
+      </c>
+      <c r="M12" s="2">
+        <v>42458</v>
       </c>
       <c r="N12" s="2">
-        <v>41449</v>
+        <v>41939</v>
       </c>
       <c r="O12" s="2">
-        <v>41672</v>
+        <v>42458</v>
       </c>
       <c r="P12">
-        <v>139</v>
+        <v>105</v>
       </c>
       <c r="Q12">
-        <v>2325</v>
+        <v>519</v>
       </c>
       <c r="R12">
-        <v>223</v>
+        <v>519</v>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>Alta Terapéutica</t>
+        </is>
+      </c>
+      <c r="T12" t="inlineStr">
+        <is>
+          <t>Alta Terapéutica</t>
+        </is>
       </c>
       <c r="U12" t="inlineStr">
         <is>
-          <t>PG-PAB</t>
+          <t>PG-PAI</t>
         </is>
       </c>
       <c r="V12">
-        <v>15880</v>
+        <v>16370</v>
       </c>
       <c r="W12">
-        <v>16103</v>
+        <v>16889</v>
       </c>
       <c r="X12">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -1364,56 +1405,53 @@
       <c r="B13">
         <v>2</v>
       </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
       <c r="D13">
         <v>0</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="F13">
+        <v>0</v>
       </c>
       <c r="G13">
-        <v>214</v>
+        <v>511</v>
       </c>
       <c r="H13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I13">
-        <v>49659</v>
+        <v>64530</v>
       </c>
       <c r="J13">
         <v>2014</v>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>137e8525aa3f79235fa8ad90913fdcbe</t>
+          <t>380d9b27915ca8873d06f71d4d74030e</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>FAMU2**071985</t>
+          <t>JUCA1**071955</t>
         </is>
       </c>
       <c r="M13" s="2">
-        <v>41791</v>
+        <v>41948</v>
       </c>
       <c r="N13" s="2">
-        <v>41458</v>
+        <v>41947</v>
       </c>
       <c r="O13" s="2">
-        <v>41791</v>
-      </c>
-      <c r="P13">
-        <v>139</v>
+        <v>41948</v>
       </c>
       <c r="Q13">
-        <v>333</v>
+        <v>1</v>
       </c>
       <c r="R13">
-        <v>333</v>
+        <v>1</v>
       </c>
       <c r="S13" t="inlineStr">
         <is>
@@ -1427,17 +1465,17 @@
       </c>
       <c r="U13" t="inlineStr">
         <is>
-          <t>PG-PAI</t>
+          <t>CALLE</t>
         </is>
       </c>
       <c r="V13">
-        <v>15889</v>
+        <v>16378</v>
       </c>
       <c r="W13">
-        <v>16222</v>
+        <v>16379</v>
       </c>
       <c r="X13">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -1450,7 +1488,7 @@
         <v>1</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -1460,69 +1498,53 @@
           <t>Si</t>
         </is>
       </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
       <c r="G14">
-        <v>6</v>
+        <v>88</v>
       </c>
       <c r="H14">
         <v>1</v>
       </c>
       <c r="I14">
-        <v>36873</v>
+        <v>89750</v>
       </c>
       <c r="J14">
-        <v>2013</v>
+        <v>2016</v>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>953090fd0a141e1cb79c86c7b209009f</t>
+          <t>a91ebc49e725f0638be44c6e17445adb</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>JOPA1**031985</t>
-        </is>
-      </c>
-      <c r="M14" s="2">
-        <v>41449</v>
+          <t>BACA1**071992</t>
+        </is>
       </c>
       <c r="N14" s="2">
-        <v>41295</v>
+        <v>42270</v>
       </c>
       <c r="O14" s="2">
-        <v>41437</v>
+        <v>42366</v>
       </c>
       <c r="P14">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="Q14">
-        <v>154</v>
+        <v>1504</v>
       </c>
       <c r="R14">
-        <v>142</v>
-      </c>
-      <c r="S14" t="inlineStr">
-        <is>
-          <t>Abandono</t>
-        </is>
-      </c>
-      <c r="T14" t="inlineStr">
-        <is>
-          <t>Abandono</t>
-        </is>
+        <v>96</v>
       </c>
       <c r="U14" t="inlineStr">
         <is>
-          <t>PG-PAB</t>
+          <t>PG-PR</t>
         </is>
       </c>
       <c r="V14">
-        <v>15726</v>
+        <v>16701</v>
       </c>
       <c r="W14">
-        <v>15868</v>
+        <v>16797</v>
       </c>
       <c r="X14">
         <v>0</v>
@@ -1538,7 +1560,7 @@
         <v>2</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -1548,69 +1570,66 @@
           <t>Si</t>
         </is>
       </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
       <c r="G15">
-        <v>6</v>
+        <v>88</v>
       </c>
       <c r="H15">
         <v>1</v>
       </c>
       <c r="I15">
-        <v>42419</v>
+        <v>94274</v>
       </c>
       <c r="J15">
-        <v>2013</v>
+        <v>2016</v>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>953090fd0a141e1cb79c86c7b209009f</t>
+          <t>a91ebc49e725f0638be44c6e17445adb</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>JOPA1**031985</t>
+          <t>BACA1**071992</t>
         </is>
       </c>
       <c r="M15" s="2">
-        <v>41607</v>
+        <v>42475</v>
       </c>
       <c r="N15" s="2">
-        <v>41431</v>
+        <v>42278</v>
       </c>
       <c r="O15" s="2">
-        <v>41607</v>
+        <v>42475</v>
       </c>
       <c r="P15">
-        <v>254</v>
+        <v>167</v>
       </c>
       <c r="Q15">
-        <v>176</v>
+        <v>197</v>
       </c>
       <c r="R15">
-        <v>176</v>
+        <v>197</v>
       </c>
       <c r="S15" t="inlineStr">
         <is>
-          <t>Alta Admnistrativa</t>
+          <t>Abandono</t>
         </is>
       </c>
       <c r="T15" t="inlineStr">
         <is>
-          <t>Alta Admnistrativa</t>
+          <t>Abandono</t>
         </is>
       </c>
       <c r="U15" t="inlineStr">
         <is>
-          <t>PG-PAI</t>
+          <t>PG-PR</t>
         </is>
       </c>
       <c r="V15">
-        <v>15862</v>
+        <v>16709</v>
       </c>
       <c r="W15">
-        <v>16038</v>
+        <v>16906</v>
       </c>
       <c r="X15">
         <v>0</v>
@@ -1626,7 +1645,7 @@
         <v>1</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1636,58 +1655,42 @@
           <t>Si</t>
         </is>
       </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
       <c r="G16">
-        <v>31</v>
+        <v>214</v>
       </c>
       <c r="H16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16">
-        <v>26804</v>
+        <v>65674</v>
       </c>
       <c r="J16">
-        <v>2012</v>
+        <v>2015</v>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>5fab3d3029d511f60544d7a58d047e5c</t>
+          <t>137e8525aa3f79235fa8ad90913fdcbe</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>GABE2**081978</t>
-        </is>
-      </c>
-      <c r="M16" s="2">
-        <v>41240</v>
+          <t>FRCA1**071985</t>
+        </is>
       </c>
       <c r="N16" s="2">
-        <v>41053</v>
+        <v>41449</v>
       </c>
       <c r="O16" s="2">
-        <v>41238</v>
+        <v>41672</v>
       </c>
       <c r="P16">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="Q16">
-        <v>187</v>
+        <v>2325</v>
       </c>
       <c r="R16">
-        <v>185</v>
-      </c>
-      <c r="S16" t="inlineStr">
-        <is>
-          <t>Derivación</t>
-        </is>
-      </c>
-      <c r="T16" t="inlineStr">
-        <is>
-          <t>Derivación</t>
-        </is>
+        <v>223</v>
       </c>
       <c r="U16" t="inlineStr">
         <is>
@@ -1695,10 +1698,10 @@
         </is>
       </c>
       <c r="V16">
-        <v>15484</v>
+        <v>15880</v>
       </c>
       <c r="W16">
-        <v>15669</v>
+        <v>16103</v>
       </c>
       <c r="X16">
         <v>0</v>
@@ -1714,79 +1717,76 @@
         <v>2</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17">
         <v>0</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Si</t>
-        </is>
-      </c>
-      <c r="F17">
-        <v>1</v>
+          <t>No</t>
+        </is>
       </c>
       <c r="G17">
-        <v>31</v>
+        <v>214</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17">
-        <v>31405</v>
+        <v>49659</v>
       </c>
       <c r="J17">
-        <v>2012</v>
+        <v>2014</v>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>5fab3d3029d511f60544d7a58d047e5c</t>
+          <t>137e8525aa3f79235fa8ad90913fdcbe</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>GABE2**081978</t>
+          <t>FAMU2**071985</t>
         </is>
       </c>
       <c r="M17" s="2">
-        <v>41260</v>
+        <v>41791</v>
       </c>
       <c r="N17" s="2">
-        <v>41207</v>
+        <v>41458</v>
       </c>
       <c r="O17" s="2">
-        <v>41238</v>
+        <v>41791</v>
       </c>
       <c r="P17">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="Q17">
-        <v>53</v>
+        <v>333</v>
       </c>
       <c r="R17">
-        <v>31</v>
+        <v>333</v>
       </c>
       <c r="S17" t="inlineStr">
         <is>
-          <t>Alta Terapéutica</t>
+          <t>Alta Admnistrativa</t>
         </is>
       </c>
       <c r="T17" t="inlineStr">
         <is>
-          <t>Alta Terapéutica</t>
+          <t>Alta Admnistrativa</t>
         </is>
       </c>
       <c r="U17" t="inlineStr">
         <is>
-          <t>PG-PR</t>
+          <t>PG-PAI</t>
         </is>
       </c>
       <c r="V17">
-        <v>15638</v>
+        <v>15889</v>
       </c>
       <c r="W17">
-        <v>15669</v>
+        <v>16222</v>
       </c>
       <c r="X17">
         <v>0</v>

</xml_diff>

<commit_message>
updating markdowns according to katie bubrinski
</commit_message>
<xml_diff>
--- a/_overlaps_feb_2020_final.xlsx
+++ b/_overlaps_feb_2020_final.xlsx
@@ -1175,7 +1175,7 @@
         </is>
       </c>
       <c r="G10">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -1200,7 +1200,7 @@
         <v>42626</v>
       </c>
       <c r="O10" s="2">
-        <v>42785</v>
+        <v>42787</v>
       </c>
       <c r="P10">
         <v>205</v>
@@ -1209,7 +1209,7 @@
         <v>1148</v>
       </c>
       <c r="R10">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="U10" t="inlineStr">
         <is>
@@ -1220,7 +1220,7 @@
         <v>17057</v>
       </c>
       <c r="W10">
-        <v>17216</v>
+        <v>17218</v>
       </c>
       <c r="X10">
         <v>1</v>
@@ -1247,7 +1247,7 @@
         </is>
       </c>
       <c r="G11">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H11">
         <v>0</v>

</xml_diff>